<commit_message>
Add clipboard support, Arrange Excel Report, Add bat file for easy use
</commit_message>
<xml_diff>
--- a/Projects/ReportJiraIssues/ReportJiraIssues/Reports/2019-12-05 Report.xlsx
+++ b/Projects/ReportJiraIssues/ReportJiraIssues/Reports/2019-12-05 Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Etion Projects\UIPath\Projects\ReportJiraIssues\ReportJiraIssues\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3024AD7B-A0B9-47F3-B8A3-F40041113C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BD86CA-DCC9-4182-92B5-404F3C74BA94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{54594EF1-188C-4305-B1B2-C4A9F379F603}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{90A3177E-BC63-4DD6-8AE0-7E01C528AA59}"/>
   </bookViews>
   <sheets>
     <sheet name="Issues By Priority And Count" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>DEVTST</t>
+  </si>
+  <si>
+    <t>Issues</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
   <si>
     <t>Critical</t>
   </si>
@@ -94,8 +115,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,82 +431,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF5708B-9CEB-4D7D-AA4C-537028FD6881}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70095FF-4FA3-41C2-8930-D162F89BDD2F}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43774</v>
+      </c>
+      <c r="C2" s="1">
+        <v>43804</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
         <v>0</v>
       </c>
     </row>
@@ -494,7 +551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C60B9B-52AA-4CF8-B7E0-D0BB6FA42F64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E41BE26-9281-48DA-992A-F5FDA1B5733E}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>